<commit_message>
import customer,laporan stok kadaluwarsa
</commit_message>
<xml_diff>
--- a/writable/template/template_import_customer.xlsx
+++ b/writable/template/template_import_customer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Apps\laragon\www\Dbig\writable\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F5FD0C-C336-4621-9375-09FC0367958E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC6A8E3-A42A-450F-925B-1E8FD92FBE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{5CDFD779-944C-41F5-A5E9-348D695BA58C}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="97">
   <si>
     <t>Kode Area</t>
   </si>
@@ -397,9 +397,6 @@
     <t>08888888888</t>
   </si>
   <si>
-    <t>JL XYZ NO.15</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Bersifat opsional, jika dikosongkan akan diisi </t>
     </r>
@@ -436,6 +433,36 @@
       </rPr>
       <t>@dbig.com</t>
     </r>
+  </si>
+  <si>
+    <t>No Rumah</t>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <t>RW</t>
+  </si>
+  <si>
+    <t>Blok Rumah</t>
+  </si>
+  <si>
+    <t>Bersifat opsional, untuk keperluan e-faktur</t>
+  </si>
+  <si>
+    <t>JL XYZ B5 NO.15</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>16</t>
   </si>
 </sst>
 </file>
@@ -554,24 +581,24 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -890,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24DEEDBE-748A-4F24-8AA6-0D07AA5DCA73}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -901,108 +928,126 @@
     <col min="1" max="1" width="16" style="2" customWidth="1"/>
     <col min="2" max="7" width="31.81640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="24.453125" style="2" customWidth="1"/>
-    <col min="9" max="10" width="22.1796875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="22.7265625" style="2" customWidth="1"/>
-    <col min="12" max="15" width="8.7265625" style="2"/>
-    <col min="16" max="16" width="17.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.7265625" style="3"/>
-    <col min="20" max="16384" width="8.7265625" style="1"/>
+    <col min="9" max="14" width="22.1796875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="22.7265625" style="2" customWidth="1"/>
+    <col min="16" max="19" width="8.7265625" style="2"/>
+    <col min="20" max="20" width="18.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.7265625" style="3"/>
+    <col min="24" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="N1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="O1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="P1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="U1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="V1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="W1" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="5" t="s">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="7"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="S1:S2"/>
+  <mergeCells count="20">
+    <mergeCell ref="W1:W2"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -1011,6 +1056,8 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1114,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD4F045-B463-48C3-BCBF-22C33D405AB3}">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="B14" sqref="B14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1130,238 +1177,276 @@
     <col min="6" max="6" width="10.90625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.08984375" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="4" customWidth="1"/>
-    <col min="10" max="10" width="15.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.90625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="11" style="4" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.90625" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.36328125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="N1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="O1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="P1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="U1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="V1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="W1" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="5" t="s">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="7"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="13"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="O3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="P3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="Q3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="R3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="S3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="10"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9" t="s">
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="8"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9" t="s">
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="U4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="V4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="S4" s="10">
+      <c r="W4" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9" t="s">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9" t="s">
+      <c r="I5" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="V5" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="S5" s="10"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="W5" s="8"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -1369,301 +1454,365 @@
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
-      <c r="I7" s="15" t="s">
+      <c r="H7" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="I7" s="11" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="I8" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="12" t="s">
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="I9" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="I10" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="I11" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="I12" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="12" t="s">
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="I13" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="J13" s="14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="8" t="s">
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B26" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="8"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="8" t="s">
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="6"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="B28" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="B22:G23"/>
-    <mergeCell ref="B24:G24"/>
+  <mergeCells count="41">
+    <mergeCell ref="B26:G27"/>
+    <mergeCell ref="B28:G28"/>
     <mergeCell ref="A7:G7"/>
     <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
     <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="B12:G12"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B14:G14"/>
     <mergeCell ref="B15:G15"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
     <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>

</xml_diff>